<commit_message>
SprintBacklog and Team member report final updates
</commit_message>
<xml_diff>
--- a/docs/deliverable2/Getana_Deliverable_2_SprintBacklog_3.xlsx
+++ b/docs/deliverable2/Getana_Deliverable_2_SprintBacklog_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45385DA7-D117-424D-84C1-1E74AD1713FC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BE1B87-66AB-474A-AC89-1CADB6E866A5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="95">
   <si>
     <t>SPRINT BACKLOG — Deliverable 1</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>51, Update SRS and UML document</t>
+  </si>
+  <si>
+    <t>Yong, Vasilis, Brody: 100%</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76DA6E3B-35E3-6241-B9CA-F55457095861}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A27" sqref="A27:XFD29"/>
     </sheetView>
   </sheetViews>
@@ -1704,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1873,6 +1876,9 @@
       <c r="F14">
         <v>5</v>
       </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">

</xml_diff>